<commit_message>
Made a map on the index page
</commit_message>
<xml_diff>
--- a/static/AG_money/caldwell_consolidates_base/pac_contrib_aug_15_17_geo.xlsx
+++ b/static/AG_money/caldwell_consolidates_base/pac_contrib_aug_15_17_geo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="8520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="totals" sheetId="4" r:id="rId1"/>
@@ -7234,7 +7234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -7349,7 +7349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U678"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>